<commit_message>
edits to plot totals excel file
</commit_message>
<xml_diff>
--- a/Plot.pram.totals.xlsx
+++ b/Plot.pram.totals.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melinakozanitas/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melinakozanitas/R projects/SOD_ecology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6CAFC9-75BB-DD40-821E-54ACEC548683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BAA682-82C7-D64D-BCA6-E262505336E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37800" yWindow="2380" windowWidth="35740" windowHeight="16540" activeTab="1" xr2:uid="{58191B99-97FB-6F4F-A154-3F95FD397D92}"/>
+    <workbookView xWindow="-37080" yWindow="480" windowWidth="35740" windowHeight="16540" activeTab="1" xr2:uid="{58191B99-97FB-6F4F-A154-3F95FD397D92}"/>
   </bookViews>
   <sheets>
     <sheet name="working" sheetId="1" r:id="rId1"/>
     <sheet name="plot totals" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2137191-00C9-4D4E-8289-86C663F07287}">
   <dimension ref="A1:BG54"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AZ1" sqref="AZ1:BG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3649,15 +3649,15 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <f>SUM(B22,E22)</f>
+        <f t="shared" ref="G22:G36" si="4">SUM(B22,E22)</f>
         <v>13</v>
       </c>
       <c r="H22">
-        <f>SUM(F22,D22,C22)</f>
+        <f t="shared" ref="H22:H36" si="5">SUM(F22,D22,C22)</f>
         <v>15</v>
       </c>
       <c r="I22">
-        <f>SUM(G22:H22)</f>
+        <f t="shared" ref="I22:I36" si="6">SUM(G22:H22)</f>
         <v>28</v>
       </c>
     </row>
@@ -3681,15 +3681,15 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <f>SUM(B23,E23)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H23">
-        <f>SUM(F23,D23,C23)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I23">
-        <f>SUM(G23:H23)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
     </row>
@@ -3713,15 +3713,15 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <f>SUM(B24,E24)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H24">
-        <f>SUM(F24,D24,C24)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="I24">
-        <f>SUM(G24:H24)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
@@ -3745,15 +3745,15 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <f>SUM(B25,E25)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="H25">
-        <f>SUM(F25,D25,C25)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="I25">
-        <f>SUM(G25:H25)</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
     </row>
@@ -3777,15 +3777,15 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <f>SUM(B26,E26)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H26">
-        <f>SUM(F26,D26,C26)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I26">
-        <f>SUM(G26:H26)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
@@ -3809,15 +3809,15 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <f>SUM(B27,E27)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="H27">
-        <f>SUM(F27,D27,C27)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I27">
-        <f>SUM(G27:H27)</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
     </row>
@@ -3841,15 +3841,15 @@
         <v>1</v>
       </c>
       <c r="G28">
-        <f>SUM(B28,E28)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="H28">
-        <f>SUM(F28,D28,C28)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="I28">
-        <f>SUM(G28:H28)</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
     </row>
@@ -3873,15 +3873,15 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <f>SUM(B29,E29)</f>
+        <f t="shared" si="4"/>
         <v>46</v>
       </c>
       <c r="H29">
-        <f>SUM(F29,D29,C29)</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="I29">
-        <f>SUM(G29:H29)</f>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
     </row>
@@ -3905,15 +3905,15 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <f>SUM(B30,E30)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H30">
-        <f>SUM(F30,D30,C30)</f>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="I30">
-        <f>SUM(G30:H30)</f>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
     </row>
@@ -3937,15 +3937,15 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <f>SUM(B31,E31)</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="H31">
-        <f>SUM(F31,D31,C31)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I31">
-        <f>SUM(G31:H31)</f>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
     </row>
@@ -3969,15 +3969,15 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <f>SUM(B32,E32)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="H32">
-        <f>SUM(F32,D32,C32)</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="I32">
-        <f>SUM(G32:H32)</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
     </row>
@@ -4001,15 +4001,15 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <f>SUM(B33,E33)</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="H33">
-        <f>SUM(F33,D33,C33)</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="I33">
-        <f>SUM(G33:H33)</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
     </row>
@@ -4033,15 +4033,15 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <f>SUM(B34,E34)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H34">
-        <f>SUM(F34,D34,C34)</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="I34">
-        <f>SUM(G34:H34)</f>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
     </row>
@@ -4065,15 +4065,15 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <f>SUM(B35,E35)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="H35">
-        <f>SUM(F35,D35,C35)</f>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="I35">
-        <f>SUM(G35:H35)</f>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
     </row>
@@ -4097,15 +4097,15 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <f>SUM(B36,E36)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="H36">
-        <f>SUM(F36,D36,C36)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I36">
-        <f>SUM(G36:H36)</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
     </row>
@@ -4190,15 +4190,15 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <f t="shared" ref="G41:G54" si="4">SUM(B41,E41)</f>
+        <f t="shared" ref="G41:G54" si="7">SUM(B41,E41)</f>
         <v>6</v>
       </c>
       <c r="H41">
-        <f t="shared" ref="H41:H54" si="5">SUM(F41,D41,C41)</f>
+        <f t="shared" ref="H41:H54" si="8">SUM(F41,D41,C41)</f>
         <v>2</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I41:I54" si="6">SUM(G41:H41)</f>
+        <f t="shared" ref="I41:I54" si="9">SUM(G41:H41)</f>
         <v>8</v>
       </c>
     </row>
@@ -4222,15 +4222,15 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
       <c r="H42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>30</v>
       </c>
     </row>
@@ -4254,15 +4254,15 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="H43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
     </row>
@@ -4286,15 +4286,15 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="I44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
     </row>
@@ -4318,15 +4318,15 @@
         <v>0</v>
       </c>
       <c r="G45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="H45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
     </row>
@@ -4350,15 +4350,15 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="H46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="I46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
     </row>
@@ -4382,15 +4382,15 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>61</v>
       </c>
       <c r="H47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="I47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
     </row>
@@ -4414,15 +4414,15 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
       <c r="H48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="I48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
     </row>
@@ -4446,15 +4446,15 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
       <c r="H49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
     </row>
@@ -4478,15 +4478,15 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="H50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="I50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
     </row>
@@ -4510,15 +4510,15 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="H51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="I51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
     </row>
@@ -4542,15 +4542,15 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="H52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="I52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
     </row>
@@ -4574,15 +4574,15 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
       <c r="H53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="I53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
     </row>
@@ -4606,15 +4606,15 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="H54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="I54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
     </row>
@@ -4626,10 +4626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D908D7C4-0AEF-534A-9A03-BF41F16B1E14}">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4994,10 +4994,10 @@
         <v>0.39642857142857141</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>6.7893587159999997</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -5035,10 +5035,10 @@
         <v>0.57333333333333336</v>
       </c>
       <c r="K10">
-        <v>15.63041567</v>
+        <v>2.377722254</v>
       </c>
       <c r="L10">
-        <v>96.666666669999998</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -5332,10 +5332,10 @@
         <v>0.44888888888888889</v>
       </c>
       <c r="K18">
-        <v>6.7893587159999997</v>
+        <v>15.63041567</v>
       </c>
       <c r="L18">
-        <v>55</v>
+        <v>96.666666669999998</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -5348,1140 +5348,1132 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K20">
-        <v>2.377722254</v>
-      </c>
-      <c r="L20">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>71</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>70</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>67</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>72</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>74</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>76</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>78</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>57</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>58</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23">
-        <v>28</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>13</v>
-      </c>
-      <c r="F23">
-        <v>13</v>
-      </c>
-      <c r="G23">
-        <v>15</v>
-      </c>
-      <c r="H23">
-        <f>(D23/C23)</f>
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f>(E23/C23)</f>
-        <v>0.4642857142857143</v>
-      </c>
-      <c r="J23">
-        <f>(F23/C23)</f>
-        <v>0.4642857142857143</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
         <v>61</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H24">
-        <f t="shared" ref="H24:H37" si="0">(D24/C24)</f>
+        <f>(D24/C24)</f>
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I37" si="1">(E24/C24)</f>
-        <v>0.625</v>
+        <f>(E24/C24)</f>
+        <v>0.4642857142857143</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24:J37" si="2">(F24/C24)</f>
-        <v>0.625</v>
+        <f>(F24/C24)</f>
+        <v>0.4642857142857143</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H38" si="0">(D25/C25)</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25:I38" si="1">(E25/C25)</f>
+        <v>0.625</v>
+      </c>
+      <c r="J25">
+        <f t="shared" ref="J25:J38" si="2">(F25/C25)</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>30</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
         <v>13</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>14</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>16</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <f t="shared" si="0"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <f t="shared" si="1"/>
         <v>0.43333333333333335</v>
       </c>
-      <c r="J25">
+      <c r="J26">
         <f t="shared" si="2"/>
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>61</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>16</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>4</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>12</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26">
+      <c r="I27">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="J26">
+      <c r="J27">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="J27">
+      <c r="J28">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
         <v>60</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>21</v>
       </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28">
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
         <v>12</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>17</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>4</v>
       </c>
-      <c r="H28">
+      <c r="H29">
         <f t="shared" si="0"/>
         <v>0.23809523809523808</v>
       </c>
-      <c r="I28">
+      <c r="I29">
         <f t="shared" si="1"/>
         <v>0.5714285714285714</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <f t="shared" si="2"/>
         <v>0.80952380952380953</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>7</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>60</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>19</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>6</v>
-      </c>
-      <c r="F29">
-        <v>6</v>
-      </c>
-      <c r="G29">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
         <v>13</v>
       </c>
-      <c r="H29">
+      <c r="H30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29">
+      <c r="I30">
         <f t="shared" si="1"/>
         <v>0.31578947368421051</v>
       </c>
-      <c r="J29">
+      <c r="J30">
         <f t="shared" si="2"/>
         <v>0.31578947368421051</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>8</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>60</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>66</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>9</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>37</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>46</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>20</v>
       </c>
-      <c r="H30">
+      <c r="H31">
         <f t="shared" si="0"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="I30">
+      <c r="I31">
         <f t="shared" si="1"/>
         <v>0.56060606060606055</v>
       </c>
-      <c r="J30">
+      <c r="J31">
         <f t="shared" si="2"/>
         <v>0.69696969696969702</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>9</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>45</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
         <v>10</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>10</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>35</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
-      <c r="J31">
+      <c r="J32">
         <f t="shared" si="2"/>
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>28</v>
       </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-      <c r="E32">
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
         <v>17</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>22</v>
       </c>
-      <c r="G32">
-        <v>6</v>
-      </c>
-      <c r="H32">
+      <c r="G33">
+        <v>6</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="0"/>
         <v>0.17857142857142858</v>
       </c>
-      <c r="I32">
+      <c r="I33">
         <f t="shared" si="1"/>
         <v>0.6071428571428571</v>
       </c>
-      <c r="J32">
+      <c r="J33">
         <f t="shared" si="2"/>
         <v>0.7857142857142857</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>11</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>61</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>13</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>6</v>
-      </c>
-      <c r="F33">
-        <v>6</v>
-      </c>
-      <c r="G33">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
         <v>7</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <f t="shared" si="1"/>
         <v>0.46153846153846156</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <f t="shared" si="2"/>
         <v>0.46153846153846156</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>12</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>61</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>24</v>
       </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34">
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
         <v>11</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>13</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>11</v>
       </c>
-      <c r="H34">
+      <c r="H35">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I34">
+      <c r="I35">
         <f t="shared" si="1"/>
         <v>0.45833333333333331</v>
       </c>
-      <c r="J34">
+      <c r="J35">
         <f t="shared" si="2"/>
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>14</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>61</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>28</v>
       </c>
-      <c r="D35" s="2">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2">
-        <v>5</v>
-      </c>
-      <c r="F35">
-        <v>5</v>
-      </c>
-      <c r="G35">
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
         <v>23</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <f t="shared" si="1"/>
         <v>0.17857142857142858</v>
       </c>
-      <c r="J35">
+      <c r="J36">
         <f t="shared" si="2"/>
         <v>0.17857142857142858</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>15</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>60</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>45</v>
       </c>
-      <c r="D36" s="2">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2">
-        <v>5</v>
-      </c>
-      <c r="F36">
-        <v>6</v>
-      </c>
-      <c r="G36">
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
         <v>39</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <f t="shared" si="0"/>
         <v>2.2222222222222223E-2</v>
       </c>
-      <c r="I36">
+      <c r="I37">
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="J36">
+      <c r="J37">
         <f t="shared" si="2"/>
         <v>0.13333333333333333</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>16</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>61</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>15</v>
       </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
         <v>12</v>
       </c>
-      <c r="F37">
+      <c r="F38">
         <v>12</v>
       </c>
-      <c r="G37">
+      <c r="G38">
         <v>3</v>
       </c>
-      <c r="H37">
+      <c r="H38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37">
+      <c r="I38">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="J37">
+      <c r="J38">
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>71</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>70</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>68</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>73</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>75</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>77</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G41" t="s">
         <v>79</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H41" t="s">
         <v>57</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I41" t="s">
         <v>58</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J41" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41">
-        <v>28</v>
-      </c>
-      <c r="D41">
-        <v>20</v>
-      </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="F41">
-        <v>22</v>
-      </c>
-      <c r="G41">
-        <v>6</v>
-      </c>
-      <c r="H41">
-        <f>(D41/C41)</f>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="I41">
-        <f>(E41/C41)</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="J41">
-        <f>(F41/C41)</f>
-        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
       </c>
       <c r="C42">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H42">
-        <f t="shared" ref="H42:H55" si="3">(D42/C42)</f>
-        <v>0.625</v>
+        <f>(D42/C42)</f>
+        <v>0.7142857142857143</v>
       </c>
       <c r="I42">
-        <f t="shared" ref="I42:I55" si="4">(E42/C42)</f>
-        <v>0.125</v>
+        <f>(E42/C42)</f>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="J42">
-        <f t="shared" ref="J42:J55" si="5">(F42/C42)</f>
-        <v>0.75</v>
+        <f>(F42/C42)</f>
+        <v>0.7857142857142857</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>6</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ref="H43:H56" si="3">(D43/C43)</f>
+        <v>0.625</v>
+      </c>
+      <c r="I43">
+        <f t="shared" ref="I43:I56" si="4">(E43/C43)</f>
+        <v>0.125</v>
+      </c>
+      <c r="J43">
+        <f t="shared" ref="J43:J56" si="5">(F43/C43)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
         <v>60</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>30</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>25</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <v>4</v>
       </c>
-      <c r="F43">
+      <c r="F44">
         <v>29</v>
       </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43">
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
         <f t="shared" si="3"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="I43">
+      <c r="I44">
         <f t="shared" si="4"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="J43">
+      <c r="J44">
         <f t="shared" si="5"/>
         <v>0.96666666666666667</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>3</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>61</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>16</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>13</v>
       </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
         <v>13</v>
       </c>
-      <c r="G44">
+      <c r="G45">
         <v>3</v>
       </c>
-      <c r="H44">
+      <c r="H45">
         <f t="shared" si="3"/>
         <v>0.8125</v>
       </c>
-      <c r="I44">
+      <c r="I45">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J44">
+      <c r="J45">
         <f t="shared" si="5"/>
         <v>0.8125</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>5</v>
-      </c>
-      <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C46">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D46">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46">
         <f t="shared" si="3"/>
-        <v>0.95238095238095233</v>
+        <v>0</v>
       </c>
       <c r="I46">
         <f t="shared" si="4"/>
-        <v>4.7619047619047616E-2</v>
+        <v>0</v>
       </c>
       <c r="J46">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
         <v>60</v>
       </c>
       <c r="C47">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D47">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G47">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <f t="shared" si="3"/>
-        <v>0.36842105263157893</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="I47">
         <f t="shared" si="4"/>
-        <v>0.10526315789473684</v>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="J47">
         <f t="shared" si="5"/>
-        <v>0.47368421052631576</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
         <v>60</v>
       </c>
       <c r="C48">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="D48">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="E48">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F48">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H48">
         <f t="shared" si="3"/>
-        <v>0.80303030303030298</v>
+        <v>0.36842105263157893</v>
       </c>
       <c r="I48">
         <f t="shared" si="4"/>
-        <v>0.12121212121212122</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="J48">
         <f t="shared" si="5"/>
-        <v>0.9242424242424242</v>
+        <v>0.47368421052631576</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49" t="s">
         <v>60</v>
       </c>
       <c r="C49">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="D49">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="E49">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F49">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="G49">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H49">
         <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
+        <v>0.80303030303030298</v>
       </c>
       <c r="I49">
         <f t="shared" si="4"/>
-        <v>0.15555555555555556</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="J49">
         <f t="shared" si="5"/>
-        <v>0.82222222222222219</v>
+        <v>0.9242424242424242</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
         <v>60</v>
       </c>
       <c r="C50">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D50">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F50">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H50">
         <f t="shared" si="3"/>
-        <v>0.9642857142857143</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I50">
         <f t="shared" si="4"/>
-        <v>3.5714285714285712E-2</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="J50">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.82222222222222219</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="G51">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <f t="shared" si="3"/>
-        <v>0.38461538461538464</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="I51">
         <f t="shared" si="4"/>
-        <v>0.15384615384615385</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="J51">
         <f t="shared" si="5"/>
-        <v>0.53846153846153844</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
         <v>61</v>
       </c>
       <c r="C52">
-        <v>24</v>
-      </c>
-      <c r="D52" s="2">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
       </c>
       <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
         <v>7</v>
       </c>
-      <c r="F52">
-        <v>13</v>
-      </c>
       <c r="G52">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H52">
         <f t="shared" si="3"/>
-        <v>0.25</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="I52">
         <f t="shared" si="4"/>
-        <v>0.29166666666666669</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="J52">
         <f t="shared" si="5"/>
-        <v>0.54166666666666663</v>
+        <v>0.53846153846153844</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
         <v>61</v>
       </c>
       <c r="C53">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D53" s="2">
-        <v>12</v>
-      </c>
-      <c r="E53" s="2">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>7</v>
       </c>
       <c r="F53">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G53">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H53">
         <f t="shared" si="3"/>
-        <v>0.42857142857142855</v>
+        <v>0.25</v>
       </c>
       <c r="I53">
         <f t="shared" si="4"/>
-        <v>0.2857142857142857</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="J53">
         <f t="shared" si="5"/>
-        <v>0.7142857142857143</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C54">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D54" s="2">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E54" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F54">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G54">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H54">
         <f t="shared" si="3"/>
-        <v>0.75555555555555554</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="I54">
         <f t="shared" si="4"/>
-        <v>0.1111111111111111</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="J54">
         <f t="shared" si="5"/>
-        <v>0.8666666666666667</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D55" s="2">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E55" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F55">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G55">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H55">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>0.75555555555555554</v>
       </c>
       <c r="I55">
         <f t="shared" si="4"/>
-        <v>6.6666666666666666E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J55">
         <f t="shared" si="5"/>
         <v>0.8666666666666667</v>
       </c>
     </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>16</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56">
+        <v>15</v>
+      </c>
+      <c r="D56" s="2">
+        <v>12</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>13</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="5"/>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:W18">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:L18">
     <sortCondition ref="B3:B18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>